<commit_message>
add plots comparing different alpha values
</commit_message>
<xml_diff>
--- a/Assignment/02_Stochastic Gradient Descent/plots.xlsx
+++ b/Assignment/02_Stochastic Gradient Descent/plots.xlsx
@@ -9,20 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="6405" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17460" windowHeight="6405" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="alpha=0.3" sheetId="4" r:id="rId4"/>
-    <sheet name="alpha=0.1" sheetId="6" r:id="rId5"/>
-    <sheet name="alpha=0.01" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="alpha=0.3" sheetId="4" r:id="rId5"/>
+    <sheet name="alpha=0.1" sheetId="6" r:id="rId6"/>
+    <sheet name="alpha=0.01" sheetId="7" r:id="rId7"/>
+    <sheet name="J(w)" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="alpha0.01" localSheetId="5">'alpha=0.01'!$A$3:$D$21</definedName>
-    <definedName name="alpha0.1" localSheetId="4">'alpha=0.1'!$A$3:$D$21</definedName>
-    <definedName name="alpha0.3" localSheetId="3">'alpha=0.3'!$A$3:$D$21</definedName>
+    <definedName name="alpha0.01" localSheetId="6">'alpha=0.01'!$A$3:$D$21</definedName>
+    <definedName name="alpha0.1" localSheetId="5">'alpha=0.1'!$A$3:$D$21</definedName>
+    <definedName name="alpha0.3" localSheetId="4">'alpha=0.3'!$A$3:$D$21</definedName>
     <definedName name="ddat" localSheetId="0">Sheet1!$B$1:$M$5</definedName>
     <definedName name="housing" localSheetId="1">Sheet3!$A$1:$C$47</definedName>
   </definedNames>
@@ -98,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>avg</t>
   </si>
@@ -141,6 +143,15 @@
   <si>
     <t>w_2</t>
   </si>
+  <si>
+    <t>α=0.3</t>
+  </si>
+  <si>
+    <t>α=0.1</t>
+  </si>
+  <si>
+    <t>α=0.01</t>
+  </si>
 </sst>
 </file>
 
@@ -175,9 +186,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -3193,6 +3205,732 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>J(w) over iterations of Gradient Descent</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'J(w)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>α=0.3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'J(w)'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'J(w)'!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.27378245447600003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26734762731900003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26706784436499997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26705554739699999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26705500682700001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.267054983064</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26705498201900002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26705498197299998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DEEE-4260-A403-D84F35125F76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'J(w)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>α=0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'J(w)'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'J(w)'!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.36119857934799998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29637860473599997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27828923705399999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27147836063800002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26880374415399999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.267746918444</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26732882044</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26716336206899999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DEEE-4260-A403-D84F35125F76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'J(w)'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>α=0.01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'J(w)'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'J(w)'!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.83841816062200003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71728340344499997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62597076064599999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55669218694099998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.50373504371599997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46290535387999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.43112073237600002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.40611272416299998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DEEE-4260-A403-D84F35125F76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="562041680"/>
+        <c:axId val="562042992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="562041680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562042992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="562042992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>J(w)</a:t>
+                </a:r>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562041680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3353,6 +4091,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
   <cs:axisTitle>
@@ -5432,6 +6210,527 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -5584,6 +6883,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3C3BBF5-0B67-4EC2-B9E3-46F6AC989CAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>585787</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81E48EAE-9F1B-4F42-9057-93153066148B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6220,8 +7560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6776,6 +8116,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D6"/>
   <sheetViews>
@@ -6860,7 +8212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -7176,7 +8528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -7492,7 +8844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -7805,4 +9157,143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0.27378245447600003</v>
+      </c>
+      <c r="C2">
+        <v>0.36119857934799998</v>
+      </c>
+      <c r="D2">
+        <v>0.83841816062200003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>0.26734762731900003</v>
+      </c>
+      <c r="C3">
+        <v>0.29637860473599997</v>
+      </c>
+      <c r="D3">
+        <v>0.71728340344499997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.26706784436499997</v>
+      </c>
+      <c r="C4">
+        <v>0.27828923705399999</v>
+      </c>
+      <c r="D4">
+        <v>0.62597076064599999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>0.26705554739699999</v>
+      </c>
+      <c r="C5">
+        <v>0.27147836063800002</v>
+      </c>
+      <c r="D5">
+        <v>0.55669218694099998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>0.26705500682700001</v>
+      </c>
+      <c r="C6">
+        <v>0.26880374415399999</v>
+      </c>
+      <c r="D6">
+        <v>0.50373504371599997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>0.267054983064</v>
+      </c>
+      <c r="C7">
+        <v>0.267746918444</v>
+      </c>
+      <c r="D7">
+        <v>0.46290535387999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>0.26705498201900002</v>
+      </c>
+      <c r="C8">
+        <v>0.26732882044</v>
+      </c>
+      <c r="D8">
+        <v>0.43112073237600002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>80</v>
+      </c>
+      <c r="B9">
+        <v>0.26705498197299998</v>
+      </c>
+      <c r="C9">
+        <v>0.26716336206899999</v>
+      </c>
+      <c r="D9">
+        <v>0.40611272416299998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finish documenting assignment 2: Regression, Gradient Descent, Stochastic Gradient Descent
</commit_message>
<xml_diff>
--- a/Assignment/02_Stochastic Gradient Descent/plots.xlsx
+++ b/Assignment/02_Stochastic Gradient Descent/plots.xlsx
@@ -3360,28 +3360,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.27378245447600003</c:v>
+                  <c:v>0.138152689877</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26734762731900003</c:v>
+                  <c:v>0.13372749736100001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.26706784436499997</c:v>
+                  <c:v>0.13353628094700001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.26705554739699999</c:v>
+                  <c:v>0.13352787738800001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.26705500682700001</c:v>
+                  <c:v>0.133527507972</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.267054983064</c:v>
+                  <c:v>0.13352749173199999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.26705498201900002</c:v>
+                  <c:v>0.13352749101799999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.26705498197299998</c:v>
+                  <c:v>0.13352749098700001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3472,28 +3472,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.36119857934799998</c:v>
+                  <c:v>0.188264900943</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29637860473599997</c:v>
+                  <c:v>0.149747664197</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27828923705399999</c:v>
+                  <c:v>0.13969745932399999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27147836063800002</c:v>
+                  <c:v>0.135954527504</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.26880374415399999</c:v>
+                  <c:v>0.13448684476</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.267746918444</c:v>
+                  <c:v>0.13390706511700001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.26732882044</c:v>
+                  <c:v>0.13367770827</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.26716336206899999</c:v>
+                  <c:v>0.13358694395000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3584,28 +3584,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.83841816062200003</c:v>
+                  <c:v>0.42627565593</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71728340344499997</c:v>
+                  <c:v>0.36395236391699998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.62597076064599999</c:v>
+                  <c:v>0.31700019542199998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55669218694099998</c:v>
+                  <c:v>0.28140239272000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.50373504371599997</c:v>
+                  <c:v>0.25421283794900001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46290535387999998</c:v>
+                  <c:v>0.23326882478399999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.43112073237600002</c:v>
+                  <c:v>0.21698105057299999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.40611272416299998</c:v>
+                  <c:v>0.20418005363200001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3755,7 +3755,7 @@
         <c:axId val="562042992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.2"/>
+          <c:min val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -9164,8 +9164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9186,13 +9186,13 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.27378245447600003</v>
+        <v>0.138152689877</v>
       </c>
       <c r="C2">
-        <v>0.36119857934799998</v>
+        <v>0.188264900943</v>
       </c>
       <c r="D2">
-        <v>0.83841816062200003</v>
+        <v>0.42627565593</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9200,13 +9200,13 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>0.26734762731900003</v>
+        <v>0.13372749736100001</v>
       </c>
       <c r="C3">
-        <v>0.29637860473599997</v>
+        <v>0.149747664197</v>
       </c>
       <c r="D3">
-        <v>0.71728340344499997</v>
+        <v>0.36395236391699998</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -9214,13 +9214,13 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>0.26706784436499997</v>
+        <v>0.13353628094700001</v>
       </c>
       <c r="C4">
-        <v>0.27828923705399999</v>
+        <v>0.13969745932399999</v>
       </c>
       <c r="D4">
-        <v>0.62597076064599999</v>
+        <v>0.31700019542199998</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -9228,13 +9228,13 @@
         <v>40</v>
       </c>
       <c r="B5">
-        <v>0.26705554739699999</v>
+        <v>0.13352787738800001</v>
       </c>
       <c r="C5">
-        <v>0.27147836063800002</v>
+        <v>0.135954527504</v>
       </c>
       <c r="D5">
-        <v>0.55669218694099998</v>
+        <v>0.28140239272000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -9242,13 +9242,13 @@
         <v>50</v>
       </c>
       <c r="B6">
-        <v>0.26705500682700001</v>
+        <v>0.133527507972</v>
       </c>
       <c r="C6">
-        <v>0.26880374415399999</v>
+        <v>0.13448684476</v>
       </c>
       <c r="D6">
-        <v>0.50373504371599997</v>
+        <v>0.25421283794900001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -9256,13 +9256,13 @@
         <v>60</v>
       </c>
       <c r="B7">
-        <v>0.267054983064</v>
+        <v>0.13352749173199999</v>
       </c>
       <c r="C7">
-        <v>0.267746918444</v>
+        <v>0.13390706511700001</v>
       </c>
       <c r="D7">
-        <v>0.46290535387999998</v>
+        <v>0.23326882478399999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -9270,13 +9270,13 @@
         <v>70</v>
       </c>
       <c r="B8">
-        <v>0.26705498201900002</v>
+        <v>0.13352749101799999</v>
       </c>
       <c r="C8">
-        <v>0.26732882044</v>
+        <v>0.13367770827</v>
       </c>
       <c r="D8">
-        <v>0.43112073237600002</v>
+        <v>0.21698105057299999</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -9284,13 +9284,13 @@
         <v>80</v>
       </c>
       <c r="B9">
-        <v>0.26705498197299998</v>
+        <v>0.13352749098700001</v>
       </c>
       <c r="C9">
-        <v>0.26716336206899999</v>
+        <v>0.13358694395000001</v>
       </c>
       <c r="D9">
-        <v>0.40611272416299998</v>
+        <v>0.20418005363200001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>